<commit_message>
created and executed test cases for free user(42),executed get support for entervpn
</commit_message>
<xml_diff>
--- a/features.xlsx
+++ b/features.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A222432-1233-4607-A21F-1C98A0399F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CD8AA3-5BF9-48A3-B987-849DAAF3A54C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="540" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="windows" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="19">
   <si>
     <t>Features of symlex vpn</t>
   </si>
@@ -101,12 +101,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -121,9 +127,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,105 +414,105 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.21875" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -524,102 +531,102 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>

</xml_diff>